<commit_message>
zaw - bugfix - home - commit
</commit_message>
<xml_diff>
--- a/documentation/02_基本設計/01_画面遷移図.xlsx
+++ b/documentation/02_基本設計/01_画面遷移図.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7755" tabRatio="791" activeTab="1"/>
+    <workbookView windowWidth="19815" windowHeight="7755" tabRatio="791"/>
   </bookViews>
   <sheets>
     <sheet name="フロー" sheetId="14" r:id="rId1"/>
@@ -79,8 +79,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -113,10 +113,11 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -131,37 +132,22 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="ＭＳ ゴシック"/>
-      <charset val="128"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -174,6 +160,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,6 +186,11 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="11"/>
@@ -227,7 +225,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="ＭＳ ゴシック"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,37 +268,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <charset val="128"/>
     </font>
   </fonts>
   <fills count="34">
@@ -295,7 +295,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,19 +379,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,31 +457,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,109 +469,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,26 +732,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -819,11 +802,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -832,49 +832,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -883,100 +883,100 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -12194,8 +12194,8 @@
   </sheetPr>
   <dimension ref="A1:BM91"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="S52" sqref="S52"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="DW48" sqref="DW48:DW49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.66666666666667" defaultRowHeight="10.5"/>
@@ -12424,10 +12424,8 @@
       <c r="BL4" s="8"/>
       <c r="BM4" s="31"/>
     </row>
-    <row r="5" spans="1:65">
+    <row r="5" spans="1:1">
       <c r="A5" s="9"/>
-      <c r="BL5" s="10"/>
-      <c r="BM5" s="32"/>
     </row>
     <row r="6" spans="1:65">
       <c r="A6" s="9"/>
@@ -13129,7 +13127,7 @@
   </sheetPr>
   <dimension ref="A1:BK73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AL64" sqref="AL64"/>
     </sheetView>
   </sheetViews>

</xml_diff>